<commit_message>
Organise samples and templates
</commit_message>
<xml_diff>
--- a/static/excel/samples/department_config.xlsx
+++ b/static/excel/samples/department_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401ACDAA-EC57-4676-8574-08933A10E857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AFF5C7-512B-4051-8A10-B9F9A0F62F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{E4E2A758-F7D2-4D95-B1D3-14046877250E}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Course Code</t>
   </si>
@@ -88,13 +88,16 @@
     <t>Department long:</t>
   </si>
   <si>
-    <t>spreadsheet_template_generic</t>
+    <t>No. of Courses:</t>
   </si>
   <si>
-    <t>summary_template_generic</t>
+    <t>XXX 000.0</t>
   </si>
   <si>
-    <t>No. of Courses:</t>
+    <t>spreadsheet_template</t>
+  </si>
+  <si>
+    <t>summary_template</t>
   </si>
 </sst>
 </file>
@@ -329,12 +332,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -824,7 +827,7 @@
   <dimension ref="A2:H150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -835,7 +838,7 @@
     <col min="4" max="4" width="10.20703125" customWidth="1"/>
     <col min="5" max="5" width="10.95703125" customWidth="1"/>
     <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="7.5390625" style="32" customWidth="1"/>
+    <col min="7" max="7" width="7.5390625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" ht="14.5" x14ac:dyDescent="0.7">
@@ -889,13 +892,13 @@
       </c>
       <c r="B6" s="24"/>
       <c r="C6" s="29"/>
-      <c r="D6" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="31"/>
+      <c r="D6" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="34"/>
       <c r="F6" s="30">
         <f>COUNT(Courses[CU])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.65">
@@ -912,7 +915,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -928,7 +931,7 @@
         <v>13</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -942,7 +945,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="33"/>
+      <c r="G11" s="32"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.65">
@@ -964,16 +967,26 @@
       <c r="F12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="34"/>
+      <c r="G12" s="33"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.65">
-      <c r="A13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>19</v>
+      </c>
       <c r="B13" s="3"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="34"/>
+      <c r="C13" s="27">
+        <v>2</v>
+      </c>
+      <c r="D13" s="27">
+        <v>1</v>
+      </c>
+      <c r="E13" s="27">
+        <v>1</v>
+      </c>
+      <c r="F13" s="27">
+        <v>0</v>
+      </c>
+      <c r="G13" s="33"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.65">
       <c r="A14" s="9"/>
@@ -982,7 +995,7 @@
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
       <c r="F14" s="28"/>
-      <c r="G14" s="34"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.65">
@@ -2075,7 +2088,7 @@
       <c r="F150" s="28"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="eFimN8n3lr+kRyjjclbcuegC+PZk/a2npPNBBovoygBHBbP8CRyw4oStElh1d2fypl5XpXGT3KofGRgDwz2MWA==" saltValue="QgmMyolreXjRaB+meTowQw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="1">
     <mergeCell ref="D6:E6"/>
   </mergeCells>

</xml_diff>